<commit_message>
adds field to trap metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/trap_metadata.xlsx
+++ b/data-raw/metadata/trap_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-knights-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF51F10B-C9E4-4270-B5E3-7FBA0F32C056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB9F2B7-1D72-4F90-A390-EC5606E2538E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="1500" windowWidth="18390" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5540" yWindow="1290" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="78">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -265,6 +265,15 @@
   </si>
   <si>
     <t>Reading on the digital rotation counter at the start of a sampling period</t>
+  </si>
+  <si>
+    <t>Date and time of day associated with the end of trap visit. Definition varies based on visitType.</t>
+  </si>
+  <si>
+    <t>2023-12-25 10:30:12</t>
+  </si>
+  <si>
+    <t>visitTime2</t>
   </si>
 </sst>
 </file>
@@ -592,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -791,28 +800,34 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
+      <c r="B5" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="5"/>
+      <c r="J5" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="K5" s="2"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
+      <c r="L5" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>76</v>
+      </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -829,10 +844,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -867,10 +882,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -903,17 +918,17 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="16" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -923,10 +938,10 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
+      <c r="J8" s="5"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -941,12 +956,12 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -979,40 +994,30 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
       <c r="I10" s="2"/>
       <c r="J10" s="3"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="3">
-        <v>0</v>
-      </c>
-      <c r="M10" s="3">
-        <v>18326</v>
-      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -1027,12 +1032,12 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>24</v>
@@ -1059,7 +1064,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="3">
-        <v>32404</v>
+        <v>18326</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1077,10 +1082,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>24</v>
@@ -1095,7 +1100,7 @@
         <v>24</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>27</v>
@@ -1107,7 +1112,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="3">
-        <v>5</v>
+        <v>32404</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1125,7 +1130,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>30</v>
@@ -1173,28 +1178,38 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="L14" s="3">
+        <v>0</v>
+      </c>
+      <c r="M14" s="3">
+        <v>5</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1211,38 +1226,28 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="2"/>
       <c r="J15" s="3"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="3">
-        <v>32.9</v>
-      </c>
-      <c r="M15" s="3">
-        <v>28700</v>
-      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1259,10 +1264,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>24</v>
@@ -1277,7 +1282,7 @@
         <v>24</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>27</v>
@@ -1286,10 +1291,10 @@
       <c r="J16" s="3"/>
       <c r="K16" s="2"/>
       <c r="L16" s="3">
-        <v>0</v>
+        <v>32.9</v>
       </c>
       <c r="M16" s="3">
-        <v>5431</v>
+        <v>28700</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1307,10 +1312,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>24</v>
@@ -1325,7 +1330,7 @@
         <v>24</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>27</v>
@@ -1334,10 +1339,10 @@
       <c r="J17" s="3"/>
       <c r="K17" s="2"/>
       <c r="L17" s="3">
-        <v>6.9</v>
+        <v>0</v>
       </c>
       <c r="M17" s="3">
-        <v>78</v>
+        <v>5431</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1355,10 +1360,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>24</v>
@@ -1373,7 +1378,7 @@
         <v>24</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>27</v>
@@ -1382,10 +1387,10 @@
       <c r="J18" s="3"/>
       <c r="K18" s="2"/>
       <c r="L18" s="3">
-        <v>0.2</v>
+        <v>6.9</v>
       </c>
       <c r="M18" s="3">
-        <v>214</v>
+        <v>78</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1403,10 +1408,10 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>24</v>
@@ -1421,7 +1426,7 @@
         <v>24</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>27</v>
@@ -1430,10 +1435,10 @@
       <c r="J19" s="3"/>
       <c r="K19" s="2"/>
       <c r="L19" s="3">
-        <v>0.42</v>
+        <v>0.2</v>
       </c>
       <c r="M19" s="3">
-        <v>1513</v>
+        <v>214</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1451,10 +1456,10 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>24</v>
@@ -1469,7 +1474,7 @@
         <v>24</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>27</v>
@@ -1478,10 +1483,10 @@
       <c r="J20" s="3"/>
       <c r="K20" s="2"/>
       <c r="L20" s="3">
-        <v>1</v>
+        <v>0.42</v>
       </c>
       <c r="M20" s="3">
-        <v>1</v>
+        <v>1513</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1499,10 +1504,10 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>24</v>
@@ -1517,7 +1522,7 @@
         <v>24</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>27</v>
@@ -1546,19 +1551,39 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="A22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="I22" s="2"/>
       <c r="J22" s="3"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="L22" s="3">
+        <v>1</v>
+      </c>
+      <c r="M22" s="3">
+        <v>1</v>
+      </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1882,7 +1907,7 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="17"/>
+      <c r="A34" s="4"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
@@ -1910,7 +1935,7 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="18"/>
+      <c r="A35" s="17"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
@@ -1938,7 +1963,7 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="17"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
@@ -1966,7 +1991,7 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="18"/>
+      <c r="A37" s="17"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
@@ -1994,7 +2019,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="4"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -2946,7 +2971,7 @@
       <c r="Z71" s="1"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="1"/>
+      <c r="A72" s="4"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="2"/>
@@ -28873,22 +28898,50 @@
       <c r="Y997" s="1"/>
       <c r="Z997" s="1"/>
     </row>
+    <row r="998" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A998" s="1"/>
+      <c r="B998" s="1"/>
+      <c r="C998" s="1"/>
+      <c r="D998" s="2"/>
+      <c r="E998" s="1"/>
+      <c r="F998" s="3"/>
+      <c r="G998" s="3"/>
+      <c r="H998" s="3"/>
+      <c r="I998" s="2"/>
+      <c r="J998" s="3"/>
+      <c r="K998" s="2"/>
+      <c r="L998" s="3"/>
+      <c r="M998" s="3"/>
+      <c r="N998" s="1"/>
+      <c r="O998" s="1"/>
+      <c r="P998" s="1"/>
+      <c r="Q998" s="1"/>
+      <c r="R998" s="1"/>
+      <c r="S998" s="1"/>
+      <c r="T998" s="1"/>
+      <c r="U998" s="1"/>
+      <c r="V998" s="1"/>
+      <c r="W998" s="1"/>
+      <c r="X998" s="1"/>
+      <c r="Y998" s="1"/>
+      <c r="Z998" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C54:C997 C1:C42" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C55:C998 C1:C43" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E997" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E998" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F997" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F998" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H997" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H998" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fixes issue with code definitions and updates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/trap_metadata.xlsx
+++ b/data-raw/metadata/trap_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2C4ABC-09F6-6B42-B263-D499FCF198EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39DC60D-13C9-BD47-9A18-F6385F4683D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67620" yWindow="500" windowWidth="29500" windowHeight="19220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32920" yWindow="740" windowWidth="29500" windowHeight="19220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="82">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -280,9 +280,6 @@
   </si>
   <si>
     <t>enumerated</t>
-  </si>
-  <si>
-    <t>ProjectDescriptionID</t>
   </si>
   <si>
     <t>2024-06-04 11:00:51</t>
@@ -629,7 +626,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -749,7 +746,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>18</v>
@@ -807,7 +804,7 @@
         <v>69</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -851,7 +848,7 @@
         <v>69</v>
       </c>
       <c r="M5" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1403,7 +1400,7 @@
         <v>24</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>27</v>
@@ -1651,7 +1648,7 @@
         <v>69</v>
       </c>
       <c r="M23" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -1695,7 +1692,7 @@
         <v>69</v>
       </c>
       <c r="M24" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -29012,7 +29009,7 @@
   <dimension ref="A1:Z872"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29065,7 +29062,7 @@
         <v>70</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>

</xml_diff>